<commit_message>
New run scripts for testing
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -8,19 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trident/Documents/CPD_local/PCP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90866FE0-D072-5B48-99FE-9E4D3CF47E93}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950F19BC-1CF2-254D-BC05-2822A92D1903}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7400" yWindow="440" windowWidth="18120" windowHeight="15020" activeTab="1" xr2:uid="{9742D917-7E45-5347-BFB1-AA01F940CEB7}"/>
+    <workbookView xWindow="25600" yWindow="-5160" windowWidth="38400" windowHeight="21160" xr2:uid="{9742D917-7E45-5347-BFB1-AA01F940CEB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Partial" sheetId="1" r:id="rId1"/>
     <sheet name="Partitions+Size" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Partial!$A$22:$G$22</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Partial!$A$22:$G$22</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Partial!$A$22:$G$22</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Partial!$A$22:$G$22</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Partial!$A$22:$G$22</definedName>
     <definedName name="part_size" localSheetId="1">'Partitions+Size'!$A$2:$C$22</definedName>
     <definedName name="steps" localSheetId="0">Partial!$A$1:$G$20</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +37,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{CDBE24C0-50F8-CF4E-BC78-8E4822CE1018}" name="part_size" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/trident/Documents/CPD_local/PCP/part_size.csv" decimal="," thousands=" " comma="1">
+    <textPr sourceFile="/Users/trident/Documents/CPD_local/PCP/part_size.csv" decimal="," thousands=" " comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -41,7 +46,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{EA5A2CE0-42B0-7C4F-8061-A92D9A46F40F}" name="steps" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/trident/Documents/CPD_local/PCP/steps.csv" decimal="," thousands=" " comma="1">
+    <textPr sourceFile="/Users/trident/Documents/CPD_local/PCP/steps.csv" decimal="," thousands=" " comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -167,118 +172,23 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Partial!$A$22:$G$22</c:f>
@@ -311,7 +221,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9F1E-2640-B857-AEF39AB380FB}"/>
+              <c16:uniqueId val="{00000000-7434-D748-97D8-F4116BF781D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -322,10 +232,118 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1971232927"/>
+        <c:axId val="1966092543"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1971232927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1966092543"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1966092543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1971232927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -334,37 +352,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1566,7 +1553,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1623,7 +1610,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1674,13 +1661,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1691,19 +1671,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -1741,7 +1714,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -3636,23 +3609,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>476764</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>68696</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>686536</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>110436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>211218</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>172349</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>147615</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{751D7F53-8E3D-204A-B4DD-3F06FABD37AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B99BBE23-5A52-3F41-8597-D28FFBE887BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4091,10 +4064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11DB6F83-8D05-3246-928B-03CDDBCD38DB}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4109,7 +4082,7 @@
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>2.9000000000000001E-2</v>
       </c>
@@ -4131,40 +4104,8 @@
       <c r="G1">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="H1">
-        <f t="shared" ref="H1:H19" si="0">SUM(A1:G1)</f>
-        <v>10577.440999999999</v>
-      </c>
-      <c r="I1">
-        <f>100*A1/H1</f>
-        <v>2.7416839290334976E-4</v>
-      </c>
-      <c r="J1">
-        <f>100*B1/H1</f>
-        <v>0.18976234421917362</v>
-      </c>
-      <c r="K1">
-        <f>100*C1/H1</f>
-        <v>4.7270412569543056E-5</v>
-      </c>
-      <c r="L1">
-        <f>100*D1/H1</f>
-        <v>80.966180761490435</v>
-      </c>
-      <c r="M1">
-        <f>100*E1/H1</f>
-        <v>1.7017348525035498E-4</v>
-      </c>
-      <c r="N1">
-        <f>100*F1/H1</f>
-        <v>18.842648235995835</v>
-      </c>
-      <c r="O1">
-        <f>100*G1/H1</f>
-        <v>9.1704600384913534E-4</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.11899999999999999</v>
       </c>
@@ -4186,40 +4127,8 @@
       <c r="G2">
         <v>7.8E-2</v>
       </c>
-      <c r="H2">
-        <f t="shared" si="0"/>
-        <v>10561.51</v>
-      </c>
-      <c r="I2">
-        <f>100*A2/H2</f>
-        <v>1.1267328251357996E-3</v>
-      </c>
-      <c r="J2">
-        <f>100*B2/H2</f>
-        <v>0.15603829376670569</v>
-      </c>
-      <c r="K2">
-        <f>100*C2/H2</f>
-        <v>3.7873372273472264E-5</v>
-      </c>
-      <c r="L2">
-        <f>100*D2/H2</f>
-        <v>81.120407971966145</v>
-      </c>
-      <c r="M2">
-        <f>100*E2/H2</f>
-        <v>1.7989851829899322E-4</v>
-      </c>
-      <c r="N2">
-        <f>100*F2/H2</f>
-        <v>18.721470698792125</v>
-      </c>
-      <c r="O2">
-        <f>100*G2/H2</f>
-        <v>7.3853075933270906E-4</v>
-      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -4241,40 +4150,8 @@
       <c r="G3">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
-        <v>10672.865</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I20" si="1">100*A3/H3</f>
-        <v>6.558688786937716E-4</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J20" si="2">100*B3/H3</f>
-        <v>0.15144012409039184</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K20" si="3">100*C3/H3</f>
-        <v>3.7478221639644093E-5</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L20" si="4">100*D3/H3</f>
-        <v>80.544165039096825</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M20" si="5">100*E3/H3</f>
-        <v>1.7802155278830943E-4</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N20" si="6">100*F3/H3</f>
-        <v>19.30287696883639</v>
-      </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O20" si="7">100*G3/H3</f>
-        <v>6.4649932328386054E-4</v>
-      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6.8000000000000005E-2</v>
       </c>
@@ -4296,40 +4173,8 @@
       <c r="G4">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>10349.055000000002</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>6.5706482379309023E-4</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="2"/>
-        <v>0.16129008880520973</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="3"/>
-        <v>5.7976307981743246E-5</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="4"/>
-        <v>82.205863240653372</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="5"/>
-        <v>1.1595261596348649E-4</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="6"/>
-        <v>17.631464901867847</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="7"/>
-        <v>5.5077492582656089E-4</v>
-      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2.8000000000000001E-2</v>
       </c>
@@ -4351,40 +4196,8 @@
       <c r="G5">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>10363.062000000002</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>2.7019041283358141E-4</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0.10535496168989433</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="3"/>
-        <v>3.8598630404797339E-5</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="4"/>
-        <v>82.085198370906198</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="5"/>
-        <v>1.2544554881559135E-4</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="6"/>
-        <v>17.808346606437361</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="7"/>
-        <v>6.6582637448275416E-4</v>
-      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.05</v>
       </c>
@@ -4406,40 +4219,8 @@
       <c r="G6">
         <v>6.2E-2</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>10388.434000000001</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>4.8130449690492324E-4</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
-        <v>0.14721179342333982</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="3"/>
-        <v>6.7382629566689267E-5</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="4"/>
-        <v>81.94767373022728</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="5"/>
-        <v>1.1551307925718158E-4</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="6"/>
-        <v>17.903853458567479</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="7"/>
-        <v>5.9681757616210482E-4</v>
-      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5.0999999999999997E-2</v>
       </c>
@@ -4461,40 +4242,8 @@
       <c r="G7">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>10240.970000000003</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>4.9799970120017914E-4</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>0.12346486709755031</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="3"/>
-        <v>3.9058800094131699E-5</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="4"/>
-        <v>82.888534972761349</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="5"/>
-        <v>1.2694110030592802E-4</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="6"/>
-        <v>16.98676980793811</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="7"/>
-        <v>5.6635260136490969E-4</v>
-      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7.9000000000000001E-2</v>
       </c>
@@ -4516,40 +4265,8 @@
       <c r="G8">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>10457.938</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>7.5540704104384631E-4</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
-        <v>0.142159955432897</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="3"/>
-        <v>3.8248457774371968E-5</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="4"/>
-        <v>81.843763082167825</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="5"/>
-        <v>6.6934801105150946E-5</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="6"/>
-        <v>18.012633083118295</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="7"/>
-        <v>5.8328898105917243E-4</v>
-      </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2.8000000000000001E-2</v>
       </c>
@@ -4571,40 +4288,8 @@
       <c r="G9">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>10404.652999999998</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>2.6911036821698916E-4</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
-        <v>0.10479926625135891</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="3"/>
-        <v>3.8444338316712732E-5</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="4"/>
-        <v>81.885671727831777</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="5"/>
-        <v>1.5377735326685093E-4</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="6"/>
-        <v>18.008481397697743</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="7"/>
-        <v>5.8627615932986912E-4</v>
-      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2.9000000000000001E-2</v>
       </c>
@@ -4626,40 +4311,8 @@
       <c r="G10">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>10480.966999999999</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>2.7669202660403385E-4</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="2"/>
-        <v>0.1132147444028781</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="3"/>
-        <v>3.8164417462625357E-5</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="4"/>
-        <v>81.673093713585772</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="5"/>
-        <v>2.0036319167878309E-4</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="6"/>
-        <v>18.212346246295787</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="7"/>
-        <v>8.3007607981210138E-4</v>
-      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3.1E-2</v>
       </c>
@@ -4681,40 +4334,8 @@
       <c r="G11">
         <v>6.2E-2</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>10268.374</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>3.0189784672821616E-4</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="2"/>
-        <v>0.16219705281478841</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="3"/>
-        <v>3.8954560868156931E-5</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="4"/>
-        <v>82.708323635270773</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="5"/>
-        <v>2.1425008477486308E-4</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="6"/>
-        <v>17.128320413728602</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="7"/>
-        <v>6.0379569345643232E-4</v>
-      </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3.5000000000000003E-2</v>
       </c>
@@ -4736,40 +4357,8 @@
       <c r="G12">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>10279.919</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>3.4046960875859045E-4</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="2"/>
-        <v>0.16147987158264576</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="3"/>
-        <v>2.9183109322164892E-5</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="4"/>
-        <v>82.404832178152375</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="5"/>
-        <v>1.1673243728865957E-4</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="6"/>
-        <v>17.432627630626271</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="7"/>
-        <v>5.739344833359095E-4</v>
-      </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2.7E-2</v>
       </c>
@@ -4791,40 +4380,8 @@
       <c r="G13">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>10501.272000000001</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>2.5711170989571548E-4</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="2"/>
-        <v>0.13162215015476217</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="3"/>
-        <v>4.761327961031768E-5</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="4"/>
-        <v>80.912007612030237</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="5"/>
-        <v>1.3331718290888952E-4</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="6"/>
-        <v>18.955227519104351</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="7"/>
-        <v>7.0467653823270157E-4</v>
-      </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8.5999999999999993E-2</v>
       </c>
@@ -4846,40 +4403,8 @@
       <c r="G14">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>10550.741</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>8.1510862601972688E-4</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="2"/>
-        <v>0.30195035590391234</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="3"/>
-        <v>5.6868043675794899E-5</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="4"/>
-        <v>80.421460445290052</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="5"/>
-        <v>1.6112612374808558E-4</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="6"/>
-        <v>19.274854723473926</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="7"/>
-        <v>7.0137253866813713E-4</v>
-      </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.123</v>
       </c>
@@ -4901,40 +4426,8 @@
       <c r="G15">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>10506.365</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
-        <v>1.1707188927854687E-3</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="2"/>
-        <v>0.19826076859123018</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="3"/>
-        <v>3.8072159114974591E-5</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="4"/>
-        <v>80.631693264035647</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="5"/>
-        <v>1.3325255690241109E-4</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="6"/>
-        <v>19.167904408422896</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="7"/>
-        <v>7.9951534141446646E-4</v>
-      </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3.6999999999999998E-2</v>
       </c>
@@ -4956,40 +4449,8 @@
       <c r="G16">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>10546.815999999999</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>3.5081677730985352E-4</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="2"/>
-        <v>0.15890103705231989</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="3"/>
-        <v>4.740767260943967E-5</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="4"/>
-        <v>80.505149611029537</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="5"/>
-        <v>1.8014915591587074E-4</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="6"/>
-        <v>19.334650381688657</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="7"/>
-        <v>7.2059662366348294E-4</v>
-      </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3.2000000000000001E-2</v>
       </c>
@@ -5011,40 +4472,8 @@
       <c r="G17">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>10533.514000000001</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
-        <v>3.0379225774038936E-4</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="2"/>
-        <v>0.16199722144006262</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="3"/>
-        <v>3.7974032217548669E-5</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="4"/>
-        <v>80.539504670521154</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="5"/>
-        <v>1.9936366914213052E-4</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="6"/>
-        <v>19.297169016911162</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="7"/>
-        <v>7.8796116851413494E-4</v>
-      </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -5066,40 +4495,8 @@
       <c r="G18">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
-        <v>10520.688</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
-        <v>3.6119310828341261E-4</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="2"/>
-        <v>0.14880205553096906</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="3"/>
-        <v>4.7525408984659558E-5</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="4"/>
-        <v>80.582562661301239</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="5"/>
-        <v>1.2356606336011485E-4</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="6"/>
-        <v>19.267276056470831</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="7"/>
-        <v>8.269421163330762E-4</v>
-      </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -5121,40 +4518,8 @@
       <c r="G19">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>10541.371999999998</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="1"/>
-        <v>5.0278085243552742E-4</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="2"/>
-        <v>0.16218951385075875</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="3"/>
-        <v>7.5891449424230574E-5</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="4"/>
-        <v>80.566647301698509</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="5"/>
-        <v>1.7075576120451874E-4</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="6"/>
-        <v>19.269692787618162</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="7"/>
-        <v>7.2096876953019033E-4</v>
-      </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8.2000000000000003E-2</v>
       </c>
@@ -5176,40 +4541,8 @@
       <c r="G20">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="H20">
-        <f>SUM(A20:G20)</f>
-        <v>10571.415000000001</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>7.7567667147680807E-4</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="2"/>
-        <v>0.26253817488008935</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="3"/>
-        <v>5.6756829620254232E-5</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="4"/>
-        <v>80.466049246955109</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="5"/>
-        <v>1.8918943206751413E-4</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="6"/>
-        <v>19.269511224372515</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="7"/>
-        <v>8.797308591139407E-4</v>
-      </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>AVERAGE(A1:A20)</f>
         <v>5.4750000000000007E-2</v>
@@ -5219,23 +4552,23 @@
         <v>16.999650000000003</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:G21" si="8">AVERAGE(C1:C20)</f>
+        <f t="shared" ref="C21:G21" si="0">AVERAGE(C1:C20)</f>
         <v>4.8000000000000013E-3</v>
       </c>
       <c r="D21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>8512.5859999999993</v>
       </c>
       <c r="E21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>1.6000000000000004E-2</v>
       </c>
       <c r="F21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>1936.134</v>
       </c>
       <c r="G21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>7.3349999999999999E-2</v>
       </c>
       <c r="H21">
@@ -5243,7 +4576,7 @@
         <v>10465.868549999999</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <f>A21*100/H21</f>
         <v>5.2312906223153362E-4</v>
@@ -5287,7 +4620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421013B2-0BC7-DA49-A412-97D0835152A2}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>

</xml_diff>